<commit_message>
Correct mistake in UC input data
</commit_message>
<xml_diff>
--- a/tests/input/unit_commitment.xlsx
+++ b/tests/input/unit_commitment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\whbles\pyaugmecon\tests\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC20EC50-2C31-4C4E-AFF3-D5B7D1E445A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86899CE-D284-4AD3-8801-19C926368FE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6420" yWindow="2910" windowWidth="24645" windowHeight="15495" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4132,18 +4132,6 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>200</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0.95</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Simplify UC time period
</commit_message>
<xml_diff>
--- a/tests/input/unit_commitment.xlsx
+++ b/tests/input/unit_commitment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\whbles\pyaugmecon\tests\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86899CE-D284-4AD3-8801-19C926368FE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E7D9F7-DF29-4EA0-8EC9-41322F808EF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="2910" windowWidth="24645" windowHeight="15495" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6420" yWindow="2910" windowWidth="24645" windowHeight="15495" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SystemDemand" sheetId="2" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="142">
   <si>
     <t>SystemDemand</t>
   </si>
@@ -461,294 +461,6 @@
   </si>
   <si>
     <t>wed-t24</t>
-  </si>
-  <si>
-    <t>thu-t1</t>
-  </si>
-  <si>
-    <t>thu-t2</t>
-  </si>
-  <si>
-    <t>thu-t3</t>
-  </si>
-  <si>
-    <t>thu-t4</t>
-  </si>
-  <si>
-    <t>thu-t5</t>
-  </si>
-  <si>
-    <t>thu-t6</t>
-  </si>
-  <si>
-    <t>thu-t7</t>
-  </si>
-  <si>
-    <t>thu-t8</t>
-  </si>
-  <si>
-    <t>thu-t9</t>
-  </si>
-  <si>
-    <t>thu-t10</t>
-  </si>
-  <si>
-    <t>thu-t11</t>
-  </si>
-  <si>
-    <t>thu-t12</t>
-  </si>
-  <si>
-    <t>thu-t13</t>
-  </si>
-  <si>
-    <t>thu-t14</t>
-  </si>
-  <si>
-    <t>thu-t15</t>
-  </si>
-  <si>
-    <t>thu-t16</t>
-  </si>
-  <si>
-    <t>thu-t17</t>
-  </si>
-  <si>
-    <t>thu-t18</t>
-  </si>
-  <si>
-    <t>thu-t19</t>
-  </si>
-  <si>
-    <t>thu-t20</t>
-  </si>
-  <si>
-    <t>thu-t21</t>
-  </si>
-  <si>
-    <t>thu-t22</t>
-  </si>
-  <si>
-    <t>thu-t23</t>
-  </si>
-  <si>
-    <t>thu-t24</t>
-  </si>
-  <si>
-    <t>fri-t1</t>
-  </si>
-  <si>
-    <t>fri-t2</t>
-  </si>
-  <si>
-    <t>fri-t3</t>
-  </si>
-  <si>
-    <t>fri-t4</t>
-  </si>
-  <si>
-    <t>fri-t5</t>
-  </si>
-  <si>
-    <t>fri-t6</t>
-  </si>
-  <si>
-    <t>fri-t7</t>
-  </si>
-  <si>
-    <t>fri-t8</t>
-  </si>
-  <si>
-    <t>fri-t9</t>
-  </si>
-  <si>
-    <t>fri-t10</t>
-  </si>
-  <si>
-    <t>fri-t11</t>
-  </si>
-  <si>
-    <t>fri-t12</t>
-  </si>
-  <si>
-    <t>fri-t13</t>
-  </si>
-  <si>
-    <t>fri-t14</t>
-  </si>
-  <si>
-    <t>fri-t15</t>
-  </si>
-  <si>
-    <t>fri-t16</t>
-  </si>
-  <si>
-    <t>fri-t17</t>
-  </si>
-  <si>
-    <t>fri-t18</t>
-  </si>
-  <si>
-    <t>fri-t19</t>
-  </si>
-  <si>
-    <t>fri-t20</t>
-  </si>
-  <si>
-    <t>fri-t21</t>
-  </si>
-  <si>
-    <t>fri-t22</t>
-  </si>
-  <si>
-    <t>fri-t23</t>
-  </si>
-  <si>
-    <t>fri-t24</t>
-  </si>
-  <si>
-    <t>sat-t1</t>
-  </si>
-  <si>
-    <t>sat-t2</t>
-  </si>
-  <si>
-    <t>sat-t3</t>
-  </si>
-  <si>
-    <t>sat-t4</t>
-  </si>
-  <si>
-    <t>sat-t5</t>
-  </si>
-  <si>
-    <t>sat-t6</t>
-  </si>
-  <si>
-    <t>sat-t7</t>
-  </si>
-  <si>
-    <t>sat-t8</t>
-  </si>
-  <si>
-    <t>sat-t9</t>
-  </si>
-  <si>
-    <t>sat-t10</t>
-  </si>
-  <si>
-    <t>sat-t11</t>
-  </si>
-  <si>
-    <t>sat-t12</t>
-  </si>
-  <si>
-    <t>sat-t13</t>
-  </si>
-  <si>
-    <t>sat-t14</t>
-  </si>
-  <si>
-    <t>sat-t15</t>
-  </si>
-  <si>
-    <t>sat-t16</t>
-  </si>
-  <si>
-    <t>sat-t17</t>
-  </si>
-  <si>
-    <t>sat-t18</t>
-  </si>
-  <si>
-    <t>sat-t19</t>
-  </si>
-  <si>
-    <t>sat-t20</t>
-  </si>
-  <si>
-    <t>sat-t21</t>
-  </si>
-  <si>
-    <t>sat-t22</t>
-  </si>
-  <si>
-    <t>sat-t23</t>
-  </si>
-  <si>
-    <t>sat-t24</t>
-  </si>
-  <si>
-    <t>sun-t1</t>
-  </si>
-  <si>
-    <t>sun-t2</t>
-  </si>
-  <si>
-    <t>sun-t3</t>
-  </si>
-  <si>
-    <t>sun-t4</t>
-  </si>
-  <si>
-    <t>sun-t5</t>
-  </si>
-  <si>
-    <t>sun-t6</t>
-  </si>
-  <si>
-    <t>sun-t7</t>
-  </si>
-  <si>
-    <t>sun-t8</t>
-  </si>
-  <si>
-    <t>sun-t9</t>
-  </si>
-  <si>
-    <t>sun-t10</t>
-  </si>
-  <si>
-    <t>sun-t11</t>
-  </si>
-  <si>
-    <t>sun-t12</t>
-  </si>
-  <si>
-    <t>sun-t13</t>
-  </si>
-  <si>
-    <t>sun-t14</t>
-  </si>
-  <si>
-    <t>sun-t15</t>
-  </si>
-  <si>
-    <t>sun-t16</t>
-  </si>
-  <si>
-    <t>sun-t17</t>
-  </si>
-  <si>
-    <t>sun-t18</t>
-  </si>
-  <si>
-    <t>sun-t19</t>
-  </si>
-  <si>
-    <t>sun-t20</t>
-  </si>
-  <si>
-    <t>sun-t21</t>
-  </si>
-  <si>
-    <t>sun-t22</t>
-  </si>
-  <si>
-    <t>sun-t23</t>
-  </si>
-  <si>
-    <t>sun-t24</t>
   </si>
   <si>
     <t>ESS2</t>
@@ -1102,8 +814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A15DE950-C5FB-4373-941F-2DB97A6028B7}">
   <dimension ref="A1:H169"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A169" sqref="A2:A169"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A74" sqref="A74:B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1838,868 +1550,388 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B74" s="2">
-        <f>0.96*H2</f>
-        <v>2428.7999999999997</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="2"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B75" s="2">
-        <f t="shared" ref="B75:B97" si="3">0.96*H3</f>
-        <v>2217.6</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="2"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B76" s="2">
-        <f t="shared" si="3"/>
-        <v>2112</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B77" s="2">
-        <f t="shared" si="3"/>
-        <v>2112</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="2"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B78" s="2">
-        <f t="shared" si="3"/>
-        <v>2006.3999999999999</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="2"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B79" s="2">
-        <f t="shared" si="3"/>
-        <v>2006.3999999999999</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="2"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B80" s="2">
-        <f t="shared" si="3"/>
-        <v>2217.6</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="2"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B81" s="2">
-        <f t="shared" si="3"/>
-        <v>2428.7999999999997</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B82" s="2">
-        <f t="shared" si="3"/>
-        <v>2640</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B83" s="2">
-        <f t="shared" si="3"/>
-        <v>2745.6000000000004</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B84" s="2">
-        <f t="shared" si="3"/>
-        <v>2851.2000000000003</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="2"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B85" s="2">
-        <f t="shared" si="3"/>
-        <v>2956.8</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="2"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B86" s="2">
-        <f t="shared" si="3"/>
-        <v>2956.8</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B87" s="2">
-        <f t="shared" si="3"/>
-        <v>2851.2000000000003</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="2"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B88" s="2">
-        <f t="shared" si="3"/>
-        <v>2745.6000000000004</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="2"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B89" s="2">
-        <f t="shared" si="3"/>
-        <v>2745.6000000000004</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="2"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B90" s="2">
-        <f t="shared" si="3"/>
-        <v>2640</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="2"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B91" s="2">
-        <f t="shared" si="3"/>
-        <v>2640</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="2"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B92" s="2">
-        <f t="shared" si="3"/>
-        <v>2851.2000000000003</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="2"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B93" s="2">
-        <f t="shared" si="3"/>
-        <v>3062.4000000000005</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="2"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B94" s="2">
-        <f t="shared" si="3"/>
-        <v>3062.4000000000005</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="2"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B95" s="2">
-        <f t="shared" si="3"/>
-        <v>2851.2000000000003</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="2"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B96" s="2">
-        <f t="shared" si="3"/>
-        <v>2640</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="2"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B97" s="2">
-        <f t="shared" si="3"/>
-        <v>2534.4</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="2"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B98" s="2">
-        <f>0.94*H2</f>
-        <v>2378.1999999999998</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="2"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B99" s="2">
-        <f t="shared" ref="B99:B121" si="4">0.94*H3</f>
-        <v>2171.4</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="2"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B100" s="2">
-        <f t="shared" si="4"/>
-        <v>2068</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="2"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B101" s="2">
-        <f t="shared" si="4"/>
-        <v>2068</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="2"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B102" s="2">
-        <f t="shared" si="4"/>
-        <v>1964.6</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="2"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B103" s="2">
-        <f t="shared" si="4"/>
-        <v>1964.6</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="2"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B104" s="2">
-        <f t="shared" si="4"/>
-        <v>2171.4</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="2"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B105" s="2">
-        <f t="shared" si="4"/>
-        <v>2378.1999999999998</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="2"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B106" s="2">
-        <f t="shared" si="4"/>
-        <v>2585</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B107" s="2">
-        <f t="shared" si="4"/>
-        <v>2688.4</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="2"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B108" s="2">
-        <f t="shared" si="4"/>
-        <v>2791.8</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="2"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B109" s="2">
-        <f t="shared" si="4"/>
-        <v>2895.2000000000003</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="2"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B110" s="2">
-        <f t="shared" si="4"/>
-        <v>2895.2000000000003</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="2"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B111" s="2">
-        <f t="shared" si="4"/>
-        <v>2791.8</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="2"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B112" s="2">
-        <f t="shared" si="4"/>
-        <v>2688.4</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="2"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B113" s="2">
-        <f t="shared" si="4"/>
-        <v>2688.4</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="2"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B114" s="2">
-        <f t="shared" si="4"/>
-        <v>2585</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="2"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B115" s="2">
-        <f t="shared" si="4"/>
-        <v>2585</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="2"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B116" s="2">
-        <f t="shared" si="4"/>
-        <v>2791.8</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="2"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B117" s="2">
-        <f t="shared" si="4"/>
-        <v>2998.6000000000004</v>
-      </c>
+      <c r="A117" s="1"/>
+      <c r="B117" s="2"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B118" s="2">
-        <f t="shared" si="4"/>
-        <v>2998.6000000000004</v>
-      </c>
+      <c r="A118" s="1"/>
+      <c r="B118" s="2"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B119" s="2">
-        <f t="shared" si="4"/>
-        <v>2791.8</v>
-      </c>
+      <c r="A119" s="1"/>
+      <c r="B119" s="2"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B120" s="2">
-        <f t="shared" si="4"/>
-        <v>2585</v>
-      </c>
+      <c r="A120" s="1"/>
+      <c r="B120" s="2"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B121" s="2">
-        <f t="shared" si="4"/>
-        <v>2481.6</v>
-      </c>
+      <c r="A121" s="1"/>
+      <c r="B121" s="2"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B122" s="2">
-        <f>0.77*H2</f>
-        <v>1948.1000000000001</v>
-      </c>
+      <c r="A122" s="1"/>
+      <c r="B122" s="2"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B123" s="2">
-        <f t="shared" ref="B123:B145" si="5">0.77*H3</f>
-        <v>1778.7</v>
-      </c>
+      <c r="A123" s="1"/>
+      <c r="B123" s="2"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B124" s="2">
-        <f t="shared" si="5"/>
-        <v>1694</v>
-      </c>
+      <c r="A124" s="1"/>
+      <c r="B124" s="2"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B125" s="2">
-        <f t="shared" si="5"/>
-        <v>1694</v>
-      </c>
+      <c r="A125" s="1"/>
+      <c r="B125" s="2"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B126" s="2">
-        <f t="shared" si="5"/>
-        <v>1609.3</v>
-      </c>
+      <c r="A126" s="1"/>
+      <c r="B126" s="2"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B127" s="2">
-        <f t="shared" si="5"/>
-        <v>1609.3</v>
-      </c>
+      <c r="A127" s="1"/>
+      <c r="B127" s="2"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B128" s="2">
-        <f t="shared" si="5"/>
-        <v>1778.7</v>
-      </c>
+      <c r="A128" s="1"/>
+      <c r="B128" s="2"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B129" s="2">
-        <f t="shared" si="5"/>
-        <v>1948.1000000000001</v>
-      </c>
+      <c r="A129" s="1"/>
+      <c r="B129" s="2"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B130" s="2">
-        <f t="shared" si="5"/>
-        <v>2117.5</v>
-      </c>
+      <c r="A130" s="1"/>
+      <c r="B130" s="2"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B131" s="2">
-        <f t="shared" si="5"/>
-        <v>2202.2000000000003</v>
-      </c>
+      <c r="A131" s="1"/>
+      <c r="B131" s="2"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B132" s="2">
-        <f t="shared" si="5"/>
-        <v>2286.9000000000005</v>
-      </c>
+      <c r="A132" s="1"/>
+      <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B133" s="2">
-        <f t="shared" si="5"/>
-        <v>2371.6000000000004</v>
-      </c>
+      <c r="A133" s="1"/>
+      <c r="B133" s="2"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B134" s="2">
-        <f t="shared" si="5"/>
-        <v>2371.6000000000004</v>
-      </c>
+      <c r="A134" s="1"/>
+      <c r="B134" s="2"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B135" s="2">
-        <f t="shared" si="5"/>
-        <v>2286.9000000000005</v>
-      </c>
+      <c r="A135" s="1"/>
+      <c r="B135" s="2"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B136" s="2">
-        <f t="shared" si="5"/>
-        <v>2202.2000000000003</v>
-      </c>
+      <c r="A136" s="1"/>
+      <c r="B136" s="2"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B137" s="2">
-        <f t="shared" si="5"/>
-        <v>2202.2000000000003</v>
-      </c>
+      <c r="A137" s="1"/>
+      <c r="B137" s="2"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B138" s="2">
-        <f t="shared" si="5"/>
-        <v>2117.5</v>
-      </c>
+      <c r="A138" s="1"/>
+      <c r="B138" s="2"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B139" s="2">
-        <f t="shared" si="5"/>
-        <v>2117.5</v>
-      </c>
+      <c r="A139" s="1"/>
+      <c r="B139" s="2"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B140" s="2">
-        <f t="shared" si="5"/>
-        <v>2286.9000000000005</v>
-      </c>
+      <c r="A140" s="1"/>
+      <c r="B140" s="2"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B141" s="2">
-        <f t="shared" si="5"/>
-        <v>2456.3000000000002</v>
-      </c>
+      <c r="A141" s="1"/>
+      <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B142" s="2">
-        <f t="shared" si="5"/>
-        <v>2456.3000000000002</v>
-      </c>
+      <c r="A142" s="1"/>
+      <c r="B142" s="2"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B143" s="2">
-        <f t="shared" si="5"/>
-        <v>2286.9000000000005</v>
-      </c>
+      <c r="A143" s="1"/>
+      <c r="B143" s="2"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B144" s="2">
-        <f t="shared" si="5"/>
-        <v>2117.5</v>
-      </c>
+      <c r="A144" s="1"/>
+      <c r="B144" s="2"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B145" s="2">
-        <f t="shared" si="5"/>
-        <v>2032.8</v>
-      </c>
+      <c r="A145" s="1"/>
+      <c r="B145" s="2"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B146" s="2">
-        <f>0.75*H2</f>
-        <v>1897.5</v>
-      </c>
+      <c r="A146" s="1"/>
+      <c r="B146" s="2"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B147" s="2">
-        <f t="shared" ref="B147:B169" si="6">0.75*H3</f>
-        <v>1732.5</v>
-      </c>
+      <c r="A147" s="1"/>
+      <c r="B147" s="2"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B148" s="2">
-        <f t="shared" si="6"/>
-        <v>1650</v>
-      </c>
+      <c r="A148" s="1"/>
+      <c r="B148" s="2"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B149" s="2">
-        <f t="shared" si="6"/>
-        <v>1650</v>
-      </c>
+      <c r="A149" s="1"/>
+      <c r="B149" s="2"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B150" s="2">
-        <f t="shared" si="6"/>
-        <v>1567.5</v>
-      </c>
+      <c r="A150" s="1"/>
+      <c r="B150" s="2"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B151" s="2">
-        <f t="shared" si="6"/>
-        <v>1567.5</v>
-      </c>
+      <c r="A151" s="1"/>
+      <c r="B151" s="2"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B152" s="2">
-        <f t="shared" si="6"/>
-        <v>1732.5</v>
-      </c>
+      <c r="A152" s="1"/>
+      <c r="B152" s="2"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B153" s="2">
-        <f t="shared" si="6"/>
-        <v>1897.5</v>
-      </c>
+      <c r="A153" s="1"/>
+      <c r="B153" s="2"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B154" s="2">
-        <f t="shared" si="6"/>
-        <v>2062.5</v>
-      </c>
+      <c r="A154" s="1"/>
+      <c r="B154" s="2"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B155" s="2">
-        <f t="shared" si="6"/>
-        <v>2145.0000000000005</v>
-      </c>
+      <c r="A155" s="1"/>
+      <c r="B155" s="2"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B156" s="2">
-        <f t="shared" si="6"/>
-        <v>2227.5000000000005</v>
-      </c>
+      <c r="A156" s="1"/>
+      <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B157" s="2">
-        <f t="shared" si="6"/>
-        <v>2310.0000000000005</v>
-      </c>
+      <c r="A157" s="1"/>
+      <c r="B157" s="2"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B158" s="2">
-        <f t="shared" si="6"/>
-        <v>2310.0000000000005</v>
-      </c>
+      <c r="A158" s="1"/>
+      <c r="B158" s="2"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B159" s="2">
-        <f t="shared" si="6"/>
-        <v>2227.5000000000005</v>
-      </c>
+      <c r="A159" s="1"/>
+      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B160" s="2">
-        <f t="shared" si="6"/>
-        <v>2145.0000000000005</v>
-      </c>
+      <c r="A160" s="1"/>
+      <c r="B160" s="2"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B161" s="2">
-        <f t="shared" si="6"/>
-        <v>2145.0000000000005</v>
-      </c>
+      <c r="A161" s="1"/>
+      <c r="B161" s="2"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B162" s="2">
-        <f t="shared" si="6"/>
-        <v>2062.5</v>
-      </c>
+      <c r="A162" s="1"/>
+      <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B163" s="2">
-        <f t="shared" si="6"/>
-        <v>2062.5</v>
-      </c>
+      <c r="A163" s="1"/>
+      <c r="B163" s="2"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B164" s="2">
-        <f t="shared" si="6"/>
-        <v>2227.5000000000005</v>
-      </c>
+      <c r="A164" s="1"/>
+      <c r="B164" s="2"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B165" s="2">
-        <f t="shared" si="6"/>
-        <v>2392.5000000000005</v>
-      </c>
+      <c r="A165" s="1"/>
+      <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B166" s="2">
-        <f t="shared" si="6"/>
-        <v>2392.5000000000005</v>
-      </c>
+      <c r="A166" s="1"/>
+      <c r="B166" s="2"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B167" s="2">
-        <f t="shared" si="6"/>
-        <v>2227.5000000000005</v>
-      </c>
+      <c r="A167" s="1"/>
+      <c r="B167" s="2"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B168" s="2">
-        <f t="shared" si="6"/>
-        <v>2062.5</v>
-      </c>
+      <c r="A168" s="1"/>
+      <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B169" s="2">
-        <f t="shared" si="6"/>
-        <v>1980</v>
-      </c>
+      <c r="A169" s="1"/>
+      <c r="B169" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2711,8 +1943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A383889-2DD6-40A0-997B-3BE66A12B465}">
   <dimension ref="A1:B169"/>
   <sheetViews>
-    <sheetView topLeftCell="A145" workbookViewId="0">
-      <selection activeCell="B146" sqref="B146:B169"/>
+    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
+      <selection activeCell="B169" sqref="A74:B169"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3300,772 +2532,388 @@
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="B74" s="2">
-        <v>0</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="2"/>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B75" s="2">
-        <v>0</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="2"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="B76" s="2">
-        <v>0</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B77" s="2">
-        <v>0</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="2"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="B78" s="2">
-        <v>0</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="2"/>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="B79" s="2">
-        <v>0</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="2"/>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="B80" s="2">
-        <v>6.4</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="2"/>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B81" s="2">
-        <v>52.8</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="B82" s="2">
-        <v>147.19999999999999</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="2"/>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B83" s="2">
-        <v>204.8</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="2"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="B84" s="2">
-        <v>224</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="2"/>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B85" s="2">
-        <v>264.8</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="2"/>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="B86" s="2">
-        <v>308.8</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="B87" s="2">
-        <v>351.2</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="2"/>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="B88" s="2">
-        <v>341.6</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="2"/>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="B89" s="2">
-        <v>284.8</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="2"/>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="B90" s="2">
-        <v>244</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="2"/>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" s="1" t="s">
-        <v>158</v>
-      </c>
-      <c r="B91" s="2">
-        <v>133.6</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="2"/>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="B92" s="2">
-        <v>44.8</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="2"/>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="B93" s="2">
-        <v>1.6</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="2"/>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="B94" s="2">
-        <v>0</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="2"/>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B95" s="2">
-        <v>0</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="2"/>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B96" s="2">
-        <v>0</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="2"/>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A97" s="1" t="s">
-        <v>164</v>
-      </c>
-      <c r="B97" s="2">
-        <v>0</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="2"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A98" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="B98" s="2">
-        <v>0</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="2"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
-        <v>166</v>
-      </c>
-      <c r="B99" s="2">
-        <v>0</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="2"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A100" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B100" s="2">
-        <v>0</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="2"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A101" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B101" s="2">
-        <v>0</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="2"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="B102" s="2">
-        <v>0</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="2"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A103" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="B103" s="2">
-        <v>0</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="2"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A104" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="B104" s="2">
-        <v>6.4</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="2"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A105" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="B105" s="2">
-        <v>52.8</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="2"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A106" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="B106" s="2">
-        <v>147.19999999999999</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A107" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="B107" s="2">
-        <v>204.8</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="2"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A108" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="B108" s="2">
-        <v>224</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="2"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A109" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="B109" s="2">
-        <v>264.8</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="2"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A110" s="1" t="s">
-        <v>177</v>
-      </c>
-      <c r="B110" s="2">
-        <v>308.8</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="2"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A111" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="B111" s="2">
-        <v>351.2</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="2"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A112" s="1" t="s">
-        <v>179</v>
-      </c>
-      <c r="B112" s="2">
-        <v>341.6</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="2"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="B113" s="2">
-        <v>284.8</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="2"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A114" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="B114" s="2">
-        <v>244</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="2"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A115" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="B115" s="2">
-        <v>133.6</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="2"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A116" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="B116" s="2">
-        <v>44.8</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="2"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A117" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="B117" s="2">
-        <v>1.6</v>
-      </c>
+      <c r="A117" s="1"/>
+      <c r="B117" s="2"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A118" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="B118" s="2">
-        <v>0</v>
-      </c>
+      <c r="A118" s="1"/>
+      <c r="B118" s="2"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A119" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="B119" s="2">
-        <v>0</v>
-      </c>
+      <c r="A119" s="1"/>
+      <c r="B119" s="2"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A120" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="B120" s="2">
-        <v>0</v>
-      </c>
+      <c r="A120" s="1"/>
+      <c r="B120" s="2"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A121" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="B121" s="2">
-        <v>0</v>
-      </c>
+      <c r="A121" s="1"/>
+      <c r="B121" s="2"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A122" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="B122" s="2">
-        <v>0</v>
-      </c>
+      <c r="A122" s="1"/>
+      <c r="B122" s="2"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A123" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="B123" s="2">
-        <v>0</v>
-      </c>
+      <c r="A123" s="1"/>
+      <c r="B123" s="2"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A124" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="B124" s="2">
-        <v>0</v>
-      </c>
+      <c r="A124" s="1"/>
+      <c r="B124" s="2"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A125" s="1" t="s">
-        <v>192</v>
-      </c>
-      <c r="B125" s="2">
-        <v>0</v>
-      </c>
+      <c r="A125" s="1"/>
+      <c r="B125" s="2"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A126" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="B126" s="2">
-        <v>0</v>
-      </c>
+      <c r="A126" s="1"/>
+      <c r="B126" s="2"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A127" s="1" t="s">
-        <v>194</v>
-      </c>
-      <c r="B127" s="2">
-        <v>0</v>
-      </c>
+      <c r="A127" s="1"/>
+      <c r="B127" s="2"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A128" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="B128" s="2">
-        <v>6.4</v>
-      </c>
+      <c r="A128" s="1"/>
+      <c r="B128" s="2"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A129" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="B129" s="2">
-        <v>52.8</v>
-      </c>
+      <c r="A129" s="1"/>
+      <c r="B129" s="2"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A130" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="B130" s="2">
-        <v>147.19999999999999</v>
-      </c>
+      <c r="A130" s="1"/>
+      <c r="B130" s="2"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A131" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="B131" s="2">
-        <v>204.8</v>
-      </c>
+      <c r="A131" s="1"/>
+      <c r="B131" s="2"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A132" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="B132" s="2">
-        <v>224</v>
-      </c>
+      <c r="A132" s="1"/>
+      <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A133" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B133" s="2">
-        <v>264.8</v>
-      </c>
+      <c r="A133" s="1"/>
+      <c r="B133" s="2"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A134" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="B134" s="2">
-        <v>308.8</v>
-      </c>
+      <c r="A134" s="1"/>
+      <c r="B134" s="2"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A135" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="B135" s="2">
-        <v>351.2</v>
-      </c>
+      <c r="A135" s="1"/>
+      <c r="B135" s="2"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A136" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="B136" s="2">
-        <v>341.6</v>
-      </c>
+      <c r="A136" s="1"/>
+      <c r="B136" s="2"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A137" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B137" s="2">
-        <v>284.8</v>
-      </c>
+      <c r="A137" s="1"/>
+      <c r="B137" s="2"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A138" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="B138" s="2">
-        <v>244</v>
-      </c>
+      <c r="A138" s="1"/>
+      <c r="B138" s="2"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A139" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B139" s="2">
-        <v>133.6</v>
-      </c>
+      <c r="A139" s="1"/>
+      <c r="B139" s="2"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A140" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B140" s="2">
-        <v>44.8</v>
-      </c>
+      <c r="A140" s="1"/>
+      <c r="B140" s="2"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A141" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B141" s="2">
-        <v>1.6</v>
-      </c>
+      <c r="A141" s="1"/>
+      <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A142" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B142" s="2">
-        <v>0</v>
-      </c>
+      <c r="A142" s="1"/>
+      <c r="B142" s="2"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A143" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B143" s="2">
-        <v>0</v>
-      </c>
+      <c r="A143" s="1"/>
+      <c r="B143" s="2"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A144" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B144" s="2">
-        <v>0</v>
-      </c>
+      <c r="A144" s="1"/>
+      <c r="B144" s="2"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A145" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="B145" s="2">
-        <v>0</v>
-      </c>
+      <c r="A145" s="1"/>
+      <c r="B145" s="2"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A146" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="B146" s="2">
-        <v>0</v>
-      </c>
+      <c r="A146" s="1"/>
+      <c r="B146" s="2"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A147" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="B147" s="2">
-        <v>0</v>
-      </c>
+      <c r="A147" s="1"/>
+      <c r="B147" s="2"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A148" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="B148" s="2">
-        <v>0</v>
-      </c>
+      <c r="A148" s="1"/>
+      <c r="B148" s="2"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A149" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="B149" s="2">
-        <v>0</v>
-      </c>
+      <c r="A149" s="1"/>
+      <c r="B149" s="2"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A150" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="B150" s="2">
-        <v>0</v>
-      </c>
+      <c r="A150" s="1"/>
+      <c r="B150" s="2"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A151" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="B151" s="2">
-        <v>0</v>
-      </c>
+      <c r="A151" s="1"/>
+      <c r="B151" s="2"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A152" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B152" s="2">
-        <v>6.4</v>
-      </c>
+      <c r="A152" s="1"/>
+      <c r="B152" s="2"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A153" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="B153" s="2">
-        <v>52.8</v>
-      </c>
+      <c r="A153" s="1"/>
+      <c r="B153" s="2"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>221</v>
-      </c>
-      <c r="B154" s="2">
-        <v>147.19999999999999</v>
-      </c>
+      <c r="A154" s="1"/>
+      <c r="B154" s="2"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A155" s="1" t="s">
-        <v>222</v>
-      </c>
-      <c r="B155" s="2">
-        <v>204.8</v>
-      </c>
+      <c r="A155" s="1"/>
+      <c r="B155" s="2"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A156" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="B156" s="2">
-        <v>224</v>
-      </c>
+      <c r="A156" s="1"/>
+      <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A157" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="B157" s="2">
-        <v>264.8</v>
-      </c>
+      <c r="A157" s="1"/>
+      <c r="B157" s="2"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A158" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="B158" s="2">
-        <v>308.8</v>
-      </c>
+      <c r="A158" s="1"/>
+      <c r="B158" s="2"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A159" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="B159" s="2">
-        <v>351.2</v>
-      </c>
+      <c r="A159" s="1"/>
+      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A160" s="1" t="s">
-        <v>227</v>
-      </c>
-      <c r="B160" s="2">
-        <v>341.6</v>
-      </c>
+      <c r="A160" s="1"/>
+      <c r="B160" s="2"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A161" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="B161" s="2">
-        <v>284.8</v>
-      </c>
+      <c r="A161" s="1"/>
+      <c r="B161" s="2"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A162" s="1" t="s">
-        <v>229</v>
-      </c>
-      <c r="B162" s="2">
-        <v>244</v>
-      </c>
+      <c r="A162" s="1"/>
+      <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A163" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="B163" s="2">
-        <v>133.6</v>
-      </c>
+      <c r="A163" s="1"/>
+      <c r="B163" s="2"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A164" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="B164" s="2">
-        <v>44.8</v>
-      </c>
+      <c r="A164" s="1"/>
+      <c r="B164" s="2"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A165" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="B165" s="2">
-        <v>1.6</v>
-      </c>
+      <c r="A165" s="1"/>
+      <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A166" s="1" t="s">
-        <v>233</v>
-      </c>
-      <c r="B166" s="2">
-        <v>0</v>
-      </c>
+      <c r="A166" s="1"/>
+      <c r="B166" s="2"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A167" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="B167" s="2">
-        <v>0</v>
-      </c>
+      <c r="A167" s="1"/>
+      <c r="B167" s="2"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A168" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="B168" s="2">
-        <v>0</v>
-      </c>
+      <c r="A168" s="1"/>
+      <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A169" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="B169" s="2">
-        <v>0</v>
-      </c>
+      <c r="A169" s="1"/>
+      <c r="B169" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4076,7 +2924,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA6DB4F6-0966-4EA6-9049-0169328E8261}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:E4"/>
     </sheetView>
   </sheetViews>
@@ -4115,7 +2963,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>237</v>
+        <v>141</v>
       </c>
       <c r="B3">
         <v>100</v>

</xml_diff>